<commit_message>
Update homeless population Shelter & Unshelter.xlsx
</commit_message>
<xml_diff>
--- a/Data/homeless population Shelter & Unshelter.xlsx
+++ b/Data/homeless population Shelter & Unshelter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/Data Scientist Program/Final Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c1abe71445d0fcf/Documents/GitHub/Homelessness-Final-Group-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{40AE9E81-6F1C-4D47-B61B-6D52D68A6B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF78C0BB-231F-4478-BB98-063E67DDD40D}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{40AE9E81-6F1C-4D47-B61B-6D52D68A6B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048491CA-5C2C-47A2-96E2-C1F5CD872858}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1E70E3BE-CA41-401A-A8CD-DC8E82FE5762}"/>
   </bookViews>
@@ -35,25 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">unshelter families with children </t>
-  </si>
-  <si>
-    <t xml:space="preserve">unshelter Individuals  </t>
-  </si>
-  <si>
-    <t>Unsheltered total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shelter families with children </t>
-  </si>
-  <si>
-    <t xml:space="preserve">shelter Individuals  </t>
-  </si>
-  <si>
-    <t>Sheltered total</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Homeless population </t>
   </si>
@@ -416,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9CDFFC-4CF4-4292-A28D-53C80AA4F884}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +412,10 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C1">
         <v>2005</v>
@@ -486,7 +468,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -538,342 +520,6 @@
       </c>
       <c r="R2">
         <v>580466</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>415366</v>
-      </c>
-      <c r="D3">
-        <v>427971</v>
-      </c>
-      <c r="E3">
-        <v>391401</v>
-      </c>
-      <c r="F3">
-        <v>386361</v>
-      </c>
-      <c r="G3">
-        <v>403308</v>
-      </c>
-      <c r="H3">
-        <v>403543</v>
-      </c>
-      <c r="I3">
-        <v>392316</v>
-      </c>
-      <c r="J3">
-        <v>390155</v>
-      </c>
-      <c r="K3">
-        <v>394698</v>
-      </c>
-      <c r="L3">
-        <v>401051</v>
-      </c>
-      <c r="M3">
-        <v>391440</v>
-      </c>
-      <c r="N3">
-        <v>373571</v>
-      </c>
-      <c r="O3">
-        <v>360867</v>
-      </c>
-      <c r="P3">
-        <v>358363</v>
-      </c>
-      <c r="Q3">
-        <v>356422</v>
-      </c>
-      <c r="R3">
-        <v>354386</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>224293</v>
-      </c>
-      <c r="E4">
-        <v>213073</v>
-      </c>
-      <c r="F4">
-        <v>204855</v>
-      </c>
-      <c r="G4">
-        <v>215995</v>
-      </c>
-      <c r="H4">
-        <v>212218</v>
-      </c>
-      <c r="I4">
-        <v>205834</v>
-      </c>
-      <c r="J4">
-        <v>199159</v>
-      </c>
-      <c r="K4">
-        <v>203127</v>
-      </c>
-      <c r="L4">
-        <v>209148</v>
-      </c>
-      <c r="M4">
-        <v>205616</v>
-      </c>
-      <c r="N4">
-        <v>198008</v>
-      </c>
-      <c r="O4">
-        <v>193144</v>
-      </c>
-      <c r="P4">
-        <v>194340</v>
-      </c>
-      <c r="Q4">
-        <v>199531</v>
-      </c>
-      <c r="R4">
-        <v>199478</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>203678</v>
-      </c>
-      <c r="E5">
-        <v>178328</v>
-      </c>
-      <c r="F5">
-        <v>181506</v>
-      </c>
-      <c r="G5">
-        <v>187313</v>
-      </c>
-      <c r="H5">
-        <v>191325</v>
-      </c>
-      <c r="I5">
-        <v>186482</v>
-      </c>
-      <c r="J5">
-        <v>190996</v>
-      </c>
-      <c r="K5">
-        <v>191571</v>
-      </c>
-      <c r="L5">
-        <v>191903</v>
-      </c>
-      <c r="M5">
-        <v>185824</v>
-      </c>
-      <c r="N5">
-        <v>175563</v>
-      </c>
-      <c r="O5">
-        <v>167723</v>
-      </c>
-      <c r="P5">
-        <v>164023</v>
-      </c>
-      <c r="Q5">
-        <v>156891</v>
-      </c>
-      <c r="R5">
-        <v>154908</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>338781</v>
-      </c>
-      <c r="D6">
-        <v>331130</v>
-      </c>
-      <c r="E6">
-        <v>255857</v>
-      </c>
-      <c r="F6">
-        <v>253423</v>
-      </c>
-      <c r="G6">
-        <v>226919</v>
-      </c>
-      <c r="H6">
-        <v>233534</v>
-      </c>
-      <c r="I6">
-        <v>231472</v>
-      </c>
-      <c r="J6">
-        <v>231398</v>
-      </c>
-      <c r="K6">
-        <v>195666</v>
-      </c>
-      <c r="L6">
-        <v>175399</v>
-      </c>
-      <c r="M6">
-        <v>173268</v>
-      </c>
-      <c r="N6">
-        <v>176357</v>
-      </c>
-      <c r="O6">
-        <v>190129</v>
-      </c>
-      <c r="P6">
-        <v>194467</v>
-      </c>
-      <c r="Q6">
-        <v>211293</v>
-      </c>
-      <c r="R6">
-        <v>226080</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>223027</v>
-      </c>
-      <c r="D7">
-        <v>228287</v>
-      </c>
-      <c r="E7">
-        <v>199627</v>
-      </c>
-      <c r="F7">
-        <v>199670</v>
-      </c>
-      <c r="G7">
-        <v>176136</v>
-      </c>
-      <c r="H7">
-        <v>182922</v>
-      </c>
-      <c r="I7">
-        <v>181779</v>
-      </c>
-      <c r="J7">
-        <v>182997</v>
-      </c>
-      <c r="K7">
-        <v>165047</v>
-      </c>
-      <c r="L7">
-        <v>151041</v>
-      </c>
-      <c r="M7">
-        <v>152806</v>
-      </c>
-      <c r="N7">
-        <v>157204</v>
-      </c>
-      <c r="O7">
-        <v>173441</v>
-      </c>
-      <c r="P7">
-        <v>178077</v>
-      </c>
-      <c r="Q7">
-        <v>196514</v>
-      </c>
-      <c r="R7">
-        <v>209413</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>115754</v>
-      </c>
-      <c r="D8">
-        <v>102843</v>
-      </c>
-      <c r="E8">
-        <v>56230</v>
-      </c>
-      <c r="F8">
-        <v>53753</v>
-      </c>
-      <c r="G8">
-        <v>50783</v>
-      </c>
-      <c r="H8">
-        <v>50612</v>
-      </c>
-      <c r="I8">
-        <v>49693</v>
-      </c>
-      <c r="J8">
-        <v>48401</v>
-      </c>
-      <c r="K8">
-        <v>30619</v>
-      </c>
-      <c r="L8">
-        <v>24358</v>
-      </c>
-      <c r="M8">
-        <v>20462</v>
-      </c>
-      <c r="N8">
-        <v>19153</v>
-      </c>
-      <c r="O8">
-        <v>16688</v>
-      </c>
-      <c r="P8">
-        <v>16390</v>
-      </c>
-      <c r="Q8">
-        <v>14779</v>
-      </c>
-      <c r="R8">
-        <v>16667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>